<commit_message>
Release: Leitura de XLS e inserção de dados em BD
</commit_message>
<xml_diff>
--- a/src/Model/Xls/teste.xlsx
+++ b/src/Model/Xls/teste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Ramos\Desktop\PDO\src\Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Ramos\Desktop\xlsreader\src\Model\Xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54037A91-3CE7-4735-91C0-570A4EDAAB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD7881A-65FB-4645-A110-23E31658D566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6765" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,53 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Guilherme Ramos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Curso</t>
   </si>
   <si>
     <t>Nome</t>
   </si>
-  <si>
-    <t>Infra</t>
-  </si>
-  <si>
-    <t>Rafael</t>
-  </si>
-  <si>
-    <r>
-      <t>Arte</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -381,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,26 +361,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>